<commit_message>
maven, last few features
</commit_message>
<xml_diff>
--- a/Details/ProjectList.xlsx
+++ b/Details/ProjectList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LF work\LF running courses\CX2002\Assignment\2024S2\data_v1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivany\courses\SC2002\SC2002-Project\Details\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021DB320-1F74-47EA-8228-03A02A2055DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED78024-5B91-4B41-8B65-18739282C33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,21 +33,9 @@
     <t>Neighborhood</t>
   </si>
   <si>
-    <t>Type 1</t>
-  </si>
-  <si>
     <t>Selling price for Type 1</t>
   </si>
   <si>
-    <t>Number of units for Type 1</t>
-  </si>
-  <si>
-    <t>Type 2</t>
-  </si>
-  <si>
-    <t>Number of units for Type 2</t>
-  </si>
-  <si>
     <t>Selling price for Type 2</t>
   </si>
   <si>
@@ -82,6 +70,18 @@
   </si>
   <si>
     <t>Daniel,Emily</t>
+  </si>
+  <si>
+    <t>Number of 2-Room</t>
+  </si>
+  <si>
+    <t>Number of 3-Room</t>
+  </si>
+  <si>
+    <t>Always 3-Room</t>
+  </si>
+  <si>
+    <t>Always 2-Room</t>
   </si>
 </sst>
 </file>
@@ -403,18 +403,18 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="9" max="10" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5546875" customWidth="1"/>
-    <col min="13" max="13" width="29.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.36328125" customWidth="1"/>
+    <col min="9" max="10" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.54296875" customWidth="1"/>
+    <col min="13" max="13" width="29.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,48 +422,48 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -472,7 +472,7 @@
         <v>350000</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G2">
         <v>3</v>
@@ -487,13 +487,13 @@
         <v>45736</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="L2">
         <v>3</v>
       </c>
       <c r="M2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>